<commit_message>
Add updated data dictionary
</commit_message>
<xml_diff>
--- a/Section3_SimulatedData/03_ModelOutput/ModelOutput_DataDictionary.xlsx
+++ b/Section3_SimulatedData/03_ModelOutput/ModelOutput_DataDictionary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Projects\InProgress\LME_DifferenceWaves&amp;LatencyERP\Data\01_SEREEGASimulation\FinalScriptsForGitHub\DiffWave\SimData_DiffWave\ExampleOutputFiles\Section3_SimulatedData_20251009\03_ModelOutput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Projects\InProgress\LME_DifferenceWaves&amp;LatencyERP\Data\FinalScriptsForGitHub\DiffWave\SimData_DiffWave\Section3_SimulatedData_20251009\03_ModelOutput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2025954-5779-4BC3-B951-7F58069E46D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23B9BAF9-89AD-4A0C-959D-B2CCDD9AC2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="9772" xr2:uid="{80C00692-9971-491C-BFCD-93A22C7EF537}"/>
   </bookViews>
@@ -146,15 +146,9 @@
     <t>Maternal sensitivity effect extracted from LME model summary</t>
   </si>
   <si>
-    <t>P-value of maternal sensitivity effect extracted from LME model summary</t>
-  </si>
-  <si>
     <t>Age effect extracted from LME model summary</t>
   </si>
   <si>
-    <t>P-value of age effect extracted from LME model summary</t>
-  </si>
-  <si>
     <t>Trial presentation number effect extracted from LME model summary</t>
   </si>
   <si>
@@ -210,6 +204,12 @@
   </si>
   <si>
     <t>Pop. (no missing trials or subjects); 0% (all subjects had at least 10 trials per condition); 6% of subjects had fewer than 10 trials per condition; 11% of subjects had fewer than 10 trials per condition; 32% of subjects had fewer than 10 trials per condition</t>
+  </si>
+  <si>
+    <t>P-value of maternal sensitivity effect extracted from LME or ANOVA model summary</t>
+  </si>
+  <si>
+    <t>P-value of age effect extracted from LME or ANOVA model summary</t>
   </si>
 </sst>
 </file>
@@ -608,8 +608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB5C7D2-B72C-4695-A6D7-8A8D6F924E0C}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -635,7 +635,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>32</v>
@@ -646,7 +646,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
@@ -657,7 +657,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>32</v>
@@ -668,7 +668,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>32</v>
@@ -682,7 +682,7 @@
         <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
@@ -690,10 +690,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
@@ -701,7 +701,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>32</v>
@@ -712,7 +712,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>32</v>
@@ -723,7 +723,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>32</v>
@@ -734,7 +734,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>32</v>
@@ -745,10 +745,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
@@ -756,10 +756,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
@@ -767,10 +767,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
@@ -778,10 +778,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
@@ -800,10 +800,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
@@ -811,7 +811,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>34</v>
@@ -822,7 +822,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>34</v>
@@ -833,7 +833,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>34</v>
@@ -844,7 +844,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>34</v>
@@ -866,7 +866,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>34</v>
@@ -877,7 +877,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>34</v>

</xml_diff>